<commit_message>
DONE WITH CLEANING YR. AND TITLE INTO TWO COLUMNS
</commit_message>
<xml_diff>
--- a/Original Excel Files/H.xlsx
+++ b/Original Excel Files/H.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BBCDE6-8057-4EEE-8F3A-EB1C49195D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="29505" yWindow="765" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,7 +277,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -341,6 +342,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -352,6 +361,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -400,7 +412,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +445,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,6 +497,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -643,369 +689,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:G44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:I37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1996</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1996</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="A5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1983</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1983</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>24</v>
+      <c r="A14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" t="s">
-        <v>24</v>
+      <c r="A15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1966</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="s">
-        <v>52</v>
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1996</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>56</v>
+      <c r="A22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="8">
+        <v>1963</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" t="s">
-        <v>27</v>
-      </c>
-    </row>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1966</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="2"/>
       <c r="B31" s="3"/>
-      <c r="C31" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1996</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" t="s">
-        <v>78</v>
-      </c>
-      <c r="G33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
+      <c r="C31" s="2"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="4">
-        <v>1963</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" t="s">
-        <v>82</v>
-      </c>
-      <c r="F37" t="s">
-        <v>83</v>
-      </c>
-      <c r="G37" t="s">
-        <v>84</v>
-      </c>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
@@ -1035,75 +1136,42 @@
       <c r="G40" s="1"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" t="s">
-        <v>13</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" t="s">
-        <v>18</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G44">
+    <sortCondition ref="A1:A44"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1115,7 +1183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>